<commit_message>
Fix Health Bar + Enemy Death + bugs fix
</commit_message>
<xml_diff>
--- a/Assets/_Core/Info pour Graph/Stats Perso PFA.xlsx
+++ b/Assets/_Core/Info pour Graph/Stats Perso PFA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets Unity\PFA_2023\Assets\_Core\Info pour Graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBEC556-C64B-4A0D-8007-8056762F79F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C696C16A-7BC5-4F52-8E54-C103FA336E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4992" yWindow="1776" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
-  <si>
-    <t>Bricoleur</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>LV</t>
   </si>
@@ -62,16 +59,13 @@
     <t>HP UP</t>
   </si>
   <si>
-    <t>Mage</t>
-  </si>
-  <si>
     <t>Asthym</t>
   </si>
   <si>
-    <t>Enemy Def</t>
+    <t>Gray</t>
   </si>
   <si>
-    <t>Test Dmg</t>
+    <t>Maj</t>
   </si>
 </sst>
 </file>
@@ -477,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,81 +486,81 @@
   <sheetData>
     <row r="1" spans="1:30" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="T1" s="2"/>
       <c r="U1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="AD1" s="2"/>
     </row>
@@ -2171,27 +2165,6 @@
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28">
-        <f>100/(100+G29)</f>
-        <v>0.5</v>
-      </c>
-      <c r="G28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <f>(C3/D28)*1</f>
-        <v>20</v>
-      </c>
-      <c r="G29">
-        <v>100</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>